<commit_message>
percobaan commin nastar 3
</commit_message>
<xml_diff>
--- a/data/Laporan Nastar3.xlsx
+++ b/data/Laporan Nastar3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sistem Management Nastar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E7F453-AF84-46CB-B0A3-CF888E8280D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391C4AF3-F9D7-40EE-971F-635D6E897E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -490,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -501,7 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2589,7 +2587,7 @@
       <c r="A56">
         <v>51</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" t="s">
         <v>126</v>
       </c>
       <c r="C56">

</xml_diff>